<commit_message>
https://kompege.ru/variant?kim=25090569 Task 18 completed
</commit_message>
<xml_diff>
--- a/25-03-25/Task-18.xlsx
+++ b/25-03-25/Task-18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHohlov\Desktop\EGE\25-03-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF569536-EB41-4DD4-97BE-C67EB6971B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C76DFE7-8189-4918-9196-833B0C3380FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +77,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +201,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -479,7 +485,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1735,79 +1741,79 @@
         <v>1093</v>
       </c>
       <c r="B22" s="4">
-        <f>MIN(A22,B23)+B1</f>
+        <f t="shared" ref="B22:B40" si="1">MIN(A22,B23)+B1</f>
         <v>1052</v>
       </c>
       <c r="C22" s="4">
-        <f>MIN(B22,C23)+C1</f>
+        <f t="shared" ref="C22:C40" si="2">MIN(B22,C23)+C1</f>
         <v>1012</v>
       </c>
       <c r="D22" s="12">
-        <f>MIN(C22,D23)+D1</f>
+        <f t="shared" ref="D22:D40" si="3">MIN(C22,D23)+D1</f>
         <v>1050</v>
       </c>
       <c r="E22" s="4">
-        <f>MIN(E23)+E1</f>
+        <f t="shared" ref="E22:E28" si="4">MIN(E23)+E1</f>
         <v>1146</v>
       </c>
       <c r="F22" s="4">
-        <f>MIN(E22,F23)+F1</f>
+        <f t="shared" ref="F22:T22" si="5">MIN(E22,F23)+F1</f>
         <v>1144</v>
       </c>
       <c r="G22" s="4">
-        <f>MIN(F22,G23)+G1</f>
+        <f t="shared" si="5"/>
         <v>1124</v>
       </c>
       <c r="H22" s="4">
-        <f>MIN(G22,H23)+H1</f>
+        <f t="shared" si="5"/>
         <v>1205</v>
       </c>
       <c r="I22" s="4">
-        <f>MIN(H22,I23)+I1</f>
+        <f t="shared" si="5"/>
         <v>1247</v>
       </c>
       <c r="J22" s="4">
-        <f>MIN(I22,J23)+J1</f>
+        <f t="shared" si="5"/>
         <v>1258</v>
       </c>
       <c r="K22" s="4">
-        <f>MIN(J22,K23)+K1</f>
+        <f t="shared" si="5"/>
         <v>1337</v>
       </c>
       <c r="L22" s="4">
-        <f>MIN(K22,L23)+L1</f>
+        <f t="shared" si="5"/>
         <v>1375</v>
       </c>
       <c r="M22" s="4">
-        <f>MIN(L22,M23)+M1</f>
+        <f t="shared" si="5"/>
         <v>1385</v>
       </c>
       <c r="N22" s="4">
-        <f>MIN(M22,N23)+N1</f>
+        <f t="shared" si="5"/>
         <v>1416</v>
       </c>
       <c r="O22" s="4">
-        <f>MIN(N22,O23)+O1</f>
+        <f t="shared" si="5"/>
         <v>1493</v>
       </c>
       <c r="P22" s="4">
-        <f>MIN(O22,P23)+P1</f>
+        <f t="shared" si="5"/>
         <v>1535</v>
       </c>
       <c r="Q22" s="4">
-        <f>MIN(P22,Q23)+Q1</f>
+        <f t="shared" si="5"/>
         <v>1546</v>
       </c>
       <c r="R22" s="4">
-        <f>MIN(Q22,R23)+R1</f>
+        <f t="shared" si="5"/>
         <v>1600</v>
       </c>
       <c r="S22" s="4">
-        <f>MIN(R22,S23)+S1</f>
+        <f t="shared" si="5"/>
         <v>1572</v>
       </c>
       <c r="T22" s="12">
-        <f>MIN(S22,T23)+T1</f>
+        <f t="shared" si="5"/>
         <v>1571</v>
       </c>
     </row>
@@ -1817,47 +1823,47 @@
         <v>1000</v>
       </c>
       <c r="B23" s="6">
-        <f>MIN(A23,B24)+B2</f>
+        <f t="shared" si="1"/>
         <v>972</v>
       </c>
       <c r="C23" s="6">
-        <f>MIN(B23,C24)+C2</f>
+        <f t="shared" si="2"/>
         <v>998</v>
       </c>
       <c r="D23" s="7">
-        <f>MIN(C23,D24)+D2</f>
+        <f t="shared" si="3"/>
         <v>1092</v>
       </c>
       <c r="E23" s="6">
-        <f>MIN(E24)+E2</f>
+        <f t="shared" si="4"/>
         <v>1077</v>
       </c>
       <c r="F23" s="6">
-        <f>MIN(E23,F24)+F2</f>
+        <f t="shared" ref="F23:L28" si="6">MIN(E23,F24)+F2</f>
         <v>1096</v>
       </c>
       <c r="G23" s="6">
-        <f>MIN(F23,G24)+G2</f>
+        <f t="shared" si="6"/>
         <v>1072</v>
       </c>
       <c r="H23" s="6">
-        <f>MIN(G23,H24)+H2</f>
+        <f t="shared" si="6"/>
         <v>1136</v>
       </c>
       <c r="I23" s="6">
-        <f>MIN(H23,I24)+I2</f>
+        <f t="shared" si="6"/>
         <v>1221</v>
       </c>
       <c r="J23" s="6">
-        <f>MIN(I23,J24)+J2</f>
+        <f t="shared" si="6"/>
         <v>1232</v>
       </c>
       <c r="K23" s="6">
-        <f>MIN(J23,K24)+K2</f>
+        <f t="shared" si="6"/>
         <v>1305</v>
       </c>
       <c r="L23" s="6">
-        <f>MIN(K23,L24)+L2</f>
+        <f t="shared" si="6"/>
         <v>1331</v>
       </c>
       <c r="M23" s="8">
@@ -1899,63 +1905,63 @@
         <v>952</v>
       </c>
       <c r="B24" s="6">
-        <f>MIN(A24,B25)+B3</f>
+        <f t="shared" si="1"/>
         <v>921</v>
       </c>
       <c r="C24" s="6">
-        <f>MIN(B24,C25)+C3</f>
+        <f t="shared" si="2"/>
         <v>932</v>
       </c>
       <c r="D24" s="7">
-        <f>MIN(C24,D25)+D3</f>
+        <f t="shared" si="3"/>
         <v>993</v>
       </c>
       <c r="E24" s="6">
-        <f>MIN(E25)+E3</f>
+        <f t="shared" si="4"/>
         <v>1007</v>
       </c>
       <c r="F24" s="6">
-        <f>MIN(E24,F25)+F3</f>
+        <f t="shared" si="6"/>
         <v>1013</v>
       </c>
       <c r="G24" s="6">
-        <f>MIN(F24,G25)+G3</f>
+        <f t="shared" si="6"/>
         <v>1003</v>
       </c>
       <c r="H24" s="6">
-        <f>MIN(G24,H25)+H3</f>
+        <f t="shared" si="6"/>
         <v>1100</v>
       </c>
       <c r="I24" s="6">
-        <f>MIN(H24,I25)+I3</f>
+        <f t="shared" si="6"/>
         <v>1160</v>
       </c>
       <c r="J24" s="6">
-        <f>MIN(I24,J25)+J3</f>
+        <f t="shared" si="6"/>
         <v>1140</v>
       </c>
       <c r="K24" s="6">
-        <f>MIN(J24,K25)+K3</f>
+        <f t="shared" si="6"/>
         <v>1238</v>
       </c>
       <c r="L24" s="6">
-        <f>MIN(K24,L25)+L3</f>
+        <f t="shared" si="6"/>
         <v>1250</v>
       </c>
       <c r="M24" s="6">
-        <f>MIN(L24,M25)+M3</f>
+        <f t="shared" ref="M24:M32" si="7">MIN(L24,M25)+M3</f>
         <v>1122</v>
       </c>
       <c r="N24" s="6">
-        <f>MIN(M24,N25)+N3</f>
+        <f t="shared" ref="N24:N32" si="8">MIN(M24,N25)+N3</f>
         <v>1182</v>
       </c>
       <c r="O24" s="6">
-        <f>MIN(N24,O25)+O3</f>
+        <f t="shared" ref="O24:O32" si="9">MIN(N24,O25)+O3</f>
         <v>1236</v>
       </c>
       <c r="P24" s="12">
-        <f>MIN(O24,P25)+P3</f>
+        <f t="shared" ref="P24:P32" si="10">MIN(O24,P25)+P3</f>
         <v>1261</v>
       </c>
       <c r="Q24" s="6">
@@ -1963,15 +1969,15 @@
         <v>1434</v>
       </c>
       <c r="R24" s="6">
-        <f>MIN(Q24,R25)+R3</f>
+        <f t="shared" ref="R24:R36" si="11">MIN(Q24,R25)+R3</f>
         <v>1472</v>
       </c>
       <c r="S24" s="6">
-        <f>MIN(R24,S25)+S3</f>
+        <f t="shared" ref="S24:S36" si="12">MIN(R24,S25)+S3</f>
         <v>1502</v>
       </c>
       <c r="T24" s="7">
-        <f>MIN(S24,T25)+T3</f>
+        <f t="shared" ref="T24:T36" si="13">MIN(S24,T25)+T3</f>
         <v>1405</v>
       </c>
     </row>
@@ -1981,63 +1987,63 @@
         <v>928</v>
       </c>
       <c r="B25" s="6">
-        <f>MIN(A25,B26)+B4</f>
+        <f t="shared" si="1"/>
         <v>860</v>
       </c>
       <c r="C25" s="6">
-        <f>MIN(B25,C26)+C4</f>
+        <f t="shared" si="2"/>
         <v>903</v>
       </c>
       <c r="D25" s="7">
-        <f>MIN(C25,D26)+D4</f>
+        <f t="shared" si="3"/>
         <v>931</v>
       </c>
       <c r="E25" s="6">
-        <f>MIN(E26)+E4</f>
+        <f t="shared" si="4"/>
         <v>977</v>
       </c>
       <c r="F25" s="6">
-        <f>MIN(E25,F26)+F4</f>
+        <f t="shared" si="6"/>
         <v>987</v>
       </c>
       <c r="G25" s="6">
-        <f>MIN(F25,G26)+G4</f>
+        <f t="shared" si="6"/>
         <v>920</v>
       </c>
       <c r="H25" s="6">
-        <f>MIN(G25,H26)+H4</f>
+        <f t="shared" si="6"/>
         <v>1003</v>
       </c>
       <c r="I25" s="6">
-        <f>MIN(H25,I26)+I4</f>
+        <f t="shared" si="6"/>
         <v>1090</v>
       </c>
       <c r="J25" s="6">
-        <f>MIN(I25,J26)+J4</f>
+        <f t="shared" si="6"/>
         <v>1122</v>
       </c>
       <c r="K25" s="6">
-        <f>MIN(J25,K26)+K4</f>
+        <f t="shared" si="6"/>
         <v>1160</v>
       </c>
       <c r="L25" s="6">
-        <f>MIN(K25,L26)+L4</f>
+        <f t="shared" si="6"/>
         <v>1204</v>
       </c>
       <c r="M25" s="6">
-        <f>MIN(L25,M26)+M4</f>
+        <f t="shared" si="7"/>
         <v>1110</v>
       </c>
       <c r="N25" s="6">
-        <f>MIN(M25,N26)+N4</f>
+        <f t="shared" si="8"/>
         <v>1148</v>
       </c>
       <c r="O25" s="6">
-        <f>MIN(N25,O26)+O4</f>
+        <f t="shared" si="9"/>
         <v>1143</v>
       </c>
       <c r="P25" s="7">
-        <f>MIN(O25,P26)+P4</f>
+        <f t="shared" si="10"/>
         <v>1223</v>
       </c>
       <c r="Q25" s="6">
@@ -2045,15 +2051,15 @@
         <v>1361</v>
       </c>
       <c r="R25" s="6">
-        <f>MIN(Q25,R26)+R4</f>
+        <f t="shared" si="11"/>
         <v>1438</v>
       </c>
       <c r="S25" s="6">
-        <f>MIN(R25,S26)+S4</f>
+        <f t="shared" si="12"/>
         <v>1412</v>
       </c>
       <c r="T25" s="7">
-        <f>MIN(S25,T26)+T4</f>
+        <f t="shared" si="13"/>
         <v>1379</v>
       </c>
     </row>
@@ -2063,63 +2069,63 @@
         <v>831</v>
       </c>
       <c r="B26" s="6">
-        <f>MIN(A26,B27)+B5</f>
+        <f t="shared" si="1"/>
         <v>833</v>
       </c>
       <c r="C26" s="6">
-        <f>MIN(B26,C27)+C5</f>
+        <f t="shared" si="2"/>
         <v>818</v>
       </c>
       <c r="D26" s="7">
-        <f>MIN(C26,D27)+D5</f>
+        <f t="shared" si="3"/>
         <v>849</v>
       </c>
       <c r="E26" s="6">
-        <f>MIN(E27)+E5</f>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
       <c r="F26" s="6">
-        <f>MIN(E26,F27)+F5</f>
+        <f t="shared" si="6"/>
         <v>891</v>
       </c>
       <c r="G26" s="6">
-        <f>MIN(F26,G27)+G5</f>
+        <f t="shared" si="6"/>
         <v>892</v>
       </c>
       <c r="H26" s="6">
-        <f>MIN(G26,H27)+H5</f>
+        <f t="shared" si="6"/>
         <v>905</v>
       </c>
       <c r="I26" s="6">
-        <f>MIN(H26,I27)+I5</f>
+        <f t="shared" si="6"/>
         <v>997</v>
       </c>
       <c r="J26" s="6">
-        <f>MIN(I26,J27)+J5</f>
+        <f t="shared" si="6"/>
         <v>1053</v>
       </c>
       <c r="K26" s="6">
-        <f>MIN(J26,K27)+K5</f>
+        <f t="shared" si="6"/>
         <v>1061</v>
       </c>
       <c r="L26" s="6">
-        <f>MIN(K26,L27)+L5</f>
+        <f t="shared" si="6"/>
         <v>1115</v>
       </c>
       <c r="M26" s="6">
-        <f>MIN(L26,M27)+M5</f>
+        <f t="shared" si="7"/>
         <v>1065</v>
       </c>
       <c r="N26" s="6">
-        <f>MIN(M26,N27)+N5</f>
+        <f t="shared" si="8"/>
         <v>1067</v>
       </c>
       <c r="O26" s="6">
-        <f>MIN(N26,O27)+O5</f>
+        <f t="shared" si="9"/>
         <v>1111</v>
       </c>
       <c r="P26" s="7">
-        <f>MIN(O26,P27)+P5</f>
+        <f t="shared" si="10"/>
         <v>1177</v>
       </c>
       <c r="Q26" s="6">
@@ -2127,15 +2133,15 @@
         <v>1296</v>
       </c>
       <c r="R26" s="6">
-        <f>MIN(Q26,R27)+R5</f>
+        <f t="shared" si="11"/>
         <v>1351</v>
       </c>
       <c r="S26" s="6">
-        <f>MIN(R26,S27)+S5</f>
+        <f t="shared" si="12"/>
         <v>1313</v>
       </c>
       <c r="T26" s="7">
-        <f>MIN(S26,T27)+T5</f>
+        <f t="shared" si="13"/>
         <v>1324</v>
       </c>
     </row>
@@ -2145,63 +2151,63 @@
         <v>767</v>
       </c>
       <c r="B27" s="6">
-        <f>MIN(A27,B28)+B6</f>
+        <f t="shared" si="1"/>
         <v>819</v>
       </c>
       <c r="C27" s="6">
-        <f>MIN(B27,C28)+C6</f>
+        <f t="shared" si="2"/>
         <v>783</v>
       </c>
       <c r="D27" s="7">
-        <f>MIN(C27,D28)+D6</f>
+        <f t="shared" si="3"/>
         <v>825</v>
       </c>
       <c r="E27" s="6">
-        <f>MIN(E28)+E6</f>
+        <f t="shared" si="4"/>
         <v>807</v>
       </c>
       <c r="F27" s="6">
-        <f>MIN(E27,F28)+F6</f>
+        <f t="shared" si="6"/>
         <v>839</v>
       </c>
       <c r="G27" s="6">
-        <f>MIN(F27,G28)+G6</f>
+        <f t="shared" si="6"/>
         <v>843</v>
       </c>
       <c r="H27" s="6">
-        <f>MIN(G27,H28)+H6</f>
+        <f t="shared" si="6"/>
         <v>925</v>
       </c>
       <c r="I27" s="6">
-        <f>MIN(H27,I28)+I6</f>
+        <f t="shared" si="6"/>
         <v>1002</v>
       </c>
       <c r="J27" s="6">
-        <f>MIN(I27,J28)+J6</f>
+        <f t="shared" si="6"/>
         <v>1001</v>
       </c>
       <c r="K27" s="6">
-        <f>MIN(J27,K28)+K6</f>
+        <f t="shared" si="6"/>
         <v>989</v>
       </c>
       <c r="L27" s="6">
-        <f>MIN(K27,L28)+L6</f>
+        <f t="shared" si="6"/>
         <v>1023</v>
       </c>
       <c r="M27" s="6">
-        <f>MIN(L27,M28)+M6</f>
+        <f t="shared" si="7"/>
         <v>1044</v>
       </c>
       <c r="N27" s="6">
-        <f>MIN(M27,N28)+N6</f>
+        <f t="shared" si="8"/>
         <v>1015</v>
       </c>
       <c r="O27" s="6">
-        <f>MIN(N27,O28)+O6</f>
+        <f t="shared" si="9"/>
         <v>1075</v>
       </c>
       <c r="P27" s="7">
-        <f>MIN(O27,P28)+P6</f>
+        <f t="shared" si="10"/>
         <v>1095</v>
       </c>
       <c r="Q27" s="6">
@@ -2209,15 +2215,15 @@
         <v>1225</v>
       </c>
       <c r="R27" s="6">
-        <f>MIN(Q27,R28)+R6</f>
+        <f t="shared" si="11"/>
         <v>1274</v>
       </c>
       <c r="S27" s="6">
-        <f>MIN(R27,S28)+S6</f>
+        <f t="shared" si="12"/>
         <v>1289</v>
       </c>
       <c r="T27" s="7">
-        <f>MIN(S27,T28)+T6</f>
+        <f t="shared" si="13"/>
         <v>1361</v>
       </c>
     </row>
@@ -2227,63 +2233,63 @@
         <v>708</v>
       </c>
       <c r="B28" s="6">
-        <f>MIN(A28,B29)+B7</f>
+        <f t="shared" si="1"/>
         <v>772</v>
       </c>
       <c r="C28" s="6">
-        <f>MIN(B28,C29)+C7</f>
+        <f t="shared" si="2"/>
         <v>732</v>
       </c>
       <c r="D28" s="7">
-        <f>MIN(C28,D29)+D7</f>
+        <f t="shared" si="3"/>
         <v>785</v>
       </c>
       <c r="E28" s="6">
-        <f>MIN(E29)+E7</f>
+        <f t="shared" si="4"/>
         <v>732</v>
       </c>
       <c r="F28" s="6">
-        <f>MIN(E28,F29)+F7</f>
+        <f t="shared" si="6"/>
         <v>743</v>
       </c>
       <c r="G28" s="6">
-        <f>MIN(F28,G29)+G7</f>
+        <f t="shared" si="6"/>
         <v>825</v>
       </c>
       <c r="H28" s="6">
-        <f>MIN(G28,H29)+H7</f>
+        <f t="shared" si="6"/>
         <v>848</v>
       </c>
       <c r="I28" s="6">
-        <f>MIN(H28,I29)+I7</f>
+        <f t="shared" si="6"/>
         <v>932</v>
       </c>
       <c r="J28" s="6">
-        <f>MIN(I28,J29)+J7</f>
+        <f t="shared" si="6"/>
         <v>934</v>
       </c>
       <c r="K28" s="6">
-        <f>MIN(J28,K29)+K7</f>
+        <f t="shared" si="6"/>
         <v>951</v>
       </c>
       <c r="L28" s="6">
-        <f>MIN(K28,L29)+L7</f>
+        <f t="shared" si="6"/>
         <v>1044</v>
       </c>
       <c r="M28" s="6">
-        <f>MIN(L28,M29)+M7</f>
+        <f t="shared" si="7"/>
         <v>991</v>
       </c>
       <c r="N28" s="6">
-        <f>MIN(M28,N29)+N7</f>
+        <f t="shared" si="8"/>
         <v>959</v>
       </c>
       <c r="O28" s="6">
-        <f>MIN(N28,O29)+O7</f>
+        <f t="shared" si="9"/>
         <v>993</v>
       </c>
       <c r="P28" s="7">
-        <f>MIN(O28,P29)+P7</f>
+        <f t="shared" si="10"/>
         <v>1008</v>
       </c>
       <c r="Q28" s="6">
@@ -2291,15 +2297,15 @@
         <v>1202</v>
       </c>
       <c r="R28" s="6">
-        <f>MIN(Q28,R29)+R7</f>
+        <f t="shared" si="11"/>
         <v>1235</v>
       </c>
       <c r="S28" s="6">
-        <f>MIN(R28,S29)+S7</f>
+        <f t="shared" si="12"/>
         <v>1245</v>
       </c>
       <c r="T28" s="7">
-        <f>MIN(S28,T29)+T7</f>
+        <f t="shared" si="13"/>
         <v>1311</v>
       </c>
     </row>
@@ -2309,23 +2315,23 @@
         <v>690</v>
       </c>
       <c r="B29" s="6">
-        <f>MIN(A29,B30)+B8</f>
+        <f t="shared" si="1"/>
         <v>724</v>
       </c>
       <c r="C29" s="6">
-        <f>MIN(B29,C30)+C8</f>
+        <f t="shared" si="2"/>
         <v>682</v>
       </c>
       <c r="D29" s="6">
-        <f>MIN(C29,D30)+D8</f>
+        <f t="shared" si="3"/>
         <v>695</v>
       </c>
       <c r="E29" s="6">
-        <f>MIN(D29,E30)+E8</f>
+        <f t="shared" ref="E29:E40" si="14">MIN(D29,E30)+E8</f>
         <v>721</v>
       </c>
       <c r="F29" s="6">
-        <f>MIN(E29,F30)+F8</f>
+        <f t="shared" ref="F29:F40" si="15">MIN(E29,F30)+F8</f>
         <v>807</v>
       </c>
       <c r="G29" s="8">
@@ -2353,35 +2359,35 @@
         <v>1003</v>
       </c>
       <c r="M29" s="6">
-        <f>MIN(L29,M30)+M8</f>
+        <f t="shared" si="7"/>
         <v>951</v>
       </c>
       <c r="N29" s="6">
-        <f>MIN(M29,N30)+N8</f>
+        <f t="shared" si="8"/>
         <v>933</v>
       </c>
       <c r="O29" s="6">
-        <f>MIN(N29,O30)+O8</f>
+        <f t="shared" si="9"/>
         <v>1027</v>
       </c>
       <c r="P29" s="6">
-        <f>MIN(O29,P30)+P8</f>
+        <f t="shared" si="10"/>
         <v>1090</v>
       </c>
       <c r="Q29" s="6">
-        <f>MIN(P29,Q30)+Q8</f>
+        <f t="shared" ref="Q29:Q36" si="16">MIN(P29,Q30)+Q8</f>
         <v>1121</v>
       </c>
       <c r="R29" s="6">
-        <f>MIN(Q29,R30)+R8</f>
+        <f t="shared" si="11"/>
         <v>1156</v>
       </c>
       <c r="S29" s="6">
-        <f>MIN(R29,S30)+S8</f>
+        <f t="shared" si="12"/>
         <v>1205</v>
       </c>
       <c r="T29" s="7">
-        <f>MIN(S29,T30)+T8</f>
+        <f t="shared" si="13"/>
         <v>1212</v>
       </c>
     </row>
@@ -2391,35 +2397,35 @@
         <v>626</v>
       </c>
       <c r="B30" s="6">
-        <f>MIN(A30,B31)+B9</f>
+        <f t="shared" si="1"/>
         <v>636</v>
       </c>
       <c r="C30" s="6">
-        <f>MIN(B30,C31)+C9</f>
+        <f t="shared" si="2"/>
         <v>668</v>
       </c>
       <c r="D30" s="6">
-        <f>MIN(C30,D31)+D9</f>
+        <f t="shared" si="3"/>
         <v>710</v>
       </c>
       <c r="E30" s="6">
-        <f>MIN(D30,E31)+E9</f>
+        <f t="shared" si="14"/>
         <v>712</v>
       </c>
       <c r="F30" s="6">
-        <f>MIN(E30,F31)+F9</f>
+        <f t="shared" si="15"/>
         <v>762</v>
       </c>
       <c r="G30" s="6">
-        <f>MIN(F30,G31)+G9</f>
+        <f t="shared" ref="G30:G40" si="17">MIN(F30,G31)+G9</f>
         <v>765</v>
       </c>
       <c r="H30" s="6">
-        <f>MIN(G30,H31)+H9</f>
+        <f t="shared" ref="H30:H40" si="18">MIN(G30,H31)+H9</f>
         <v>835</v>
       </c>
       <c r="I30" s="12">
-        <f>MIN(H30,I31)+I9</f>
+        <f t="shared" ref="I30:I40" si="19">MIN(H30,I31)+I9</f>
         <v>903</v>
       </c>
       <c r="J30" s="6">
@@ -2427,43 +2433,43 @@
         <v>864</v>
       </c>
       <c r="K30" s="6">
-        <f>MIN(J30,K31)+K9</f>
+        <f t="shared" ref="K30:L36" si="20">MIN(J30,K31)+K9</f>
         <v>957</v>
       </c>
       <c r="L30" s="6">
-        <f>MIN(K30,L31)+L9</f>
+        <f t="shared" si="20"/>
         <v>972</v>
       </c>
       <c r="M30" s="6">
-        <f>MIN(L30,M31)+M9</f>
+        <f t="shared" si="7"/>
         <v>879</v>
       </c>
       <c r="N30" s="6">
-        <f>MIN(M30,N31)+N9</f>
+        <f t="shared" si="8"/>
         <v>900</v>
       </c>
       <c r="O30" s="6">
-        <f>MIN(N30,O31)+O9</f>
+        <f t="shared" si="9"/>
         <v>944</v>
       </c>
       <c r="P30" s="6">
-        <f>MIN(O30,P31)+P9</f>
+        <f t="shared" si="10"/>
         <v>1034</v>
       </c>
       <c r="Q30" s="6">
-        <f>MIN(P30,Q31)+Q9</f>
+        <f t="shared" si="16"/>
         <v>1062</v>
       </c>
       <c r="R30" s="6">
-        <f>MIN(Q30,R31)+R9</f>
+        <f t="shared" si="11"/>
         <v>1091</v>
       </c>
       <c r="S30" s="6">
-        <f>MIN(R30,S31)+S9</f>
+        <f t="shared" si="12"/>
         <v>1150</v>
       </c>
       <c r="T30" s="7">
-        <f>MIN(S30,T31)+T9</f>
+        <f t="shared" si="13"/>
         <v>1192</v>
       </c>
     </row>
@@ -2473,35 +2479,35 @@
         <v>611</v>
       </c>
       <c r="B31" s="6">
-        <f>MIN(A31,B32)+B10</f>
+        <f t="shared" si="1"/>
         <v>571</v>
       </c>
       <c r="C31" s="6">
-        <f>MIN(B31,C32)+C10</f>
+        <f t="shared" si="2"/>
         <v>596</v>
       </c>
       <c r="D31" s="6">
-        <f>MIN(C31,D32)+D10</f>
+        <f t="shared" si="3"/>
         <v>641</v>
       </c>
       <c r="E31" s="6">
-        <f>MIN(D31,E32)+E10</f>
+        <f t="shared" si="14"/>
         <v>684</v>
       </c>
       <c r="F31" s="6">
-        <f>MIN(E31,F32)+F10</f>
+        <f t="shared" si="15"/>
         <v>705</v>
       </c>
       <c r="G31" s="6">
-        <f>MIN(F31,G32)+G10</f>
+        <f t="shared" si="17"/>
         <v>740</v>
       </c>
       <c r="H31" s="6">
-        <f>MIN(G31,H32)+H10</f>
+        <f t="shared" si="18"/>
         <v>770</v>
       </c>
       <c r="I31" s="7">
-        <f>MIN(H31,I32)+I10</f>
+        <f t="shared" si="19"/>
         <v>807</v>
       </c>
       <c r="J31" s="6">
@@ -2509,43 +2515,43 @@
         <v>837</v>
       </c>
       <c r="K31" s="6">
-        <f>MIN(J31,K32)+K10</f>
+        <f t="shared" si="20"/>
         <v>894</v>
       </c>
       <c r="L31" s="6">
-        <f>MIN(K31,L32)+L10</f>
+        <f t="shared" si="20"/>
         <v>946</v>
       </c>
       <c r="M31" s="6">
-        <f>MIN(L31,M32)+M10</f>
+        <f t="shared" si="7"/>
         <v>867</v>
       </c>
       <c r="N31" s="6">
-        <f>MIN(M31,N32)+N10</f>
+        <f t="shared" si="8"/>
         <v>938</v>
       </c>
       <c r="O31" s="6">
-        <f>MIN(N31,O32)+O10</f>
+        <f t="shared" si="9"/>
         <v>961</v>
       </c>
       <c r="P31" s="6">
-        <f>MIN(O31,P32)+P10</f>
+        <f t="shared" si="10"/>
         <v>994</v>
       </c>
       <c r="Q31" s="6">
-        <f>MIN(P31,Q32)+Q10</f>
+        <f t="shared" si="16"/>
         <v>1040</v>
       </c>
       <c r="R31" s="6">
-        <f>MIN(Q31,R32)+R10</f>
+        <f t="shared" si="11"/>
         <v>1085</v>
       </c>
       <c r="S31" s="6">
-        <f>MIN(R31,S32)+S10</f>
+        <f t="shared" si="12"/>
         <v>1133</v>
       </c>
       <c r="T31" s="7">
-        <f>MIN(S31,T32)+T10</f>
+        <f t="shared" si="13"/>
         <v>1211</v>
       </c>
     </row>
@@ -2555,35 +2561,35 @@
         <v>558</v>
       </c>
       <c r="B32" s="6">
-        <f>MIN(A32,B33)+B11</f>
+        <f t="shared" si="1"/>
         <v>523</v>
       </c>
       <c r="C32" s="6">
-        <f>MIN(B32,C33)+C11</f>
+        <f t="shared" si="2"/>
         <v>562</v>
       </c>
       <c r="D32" s="6">
-        <f>MIN(C32,D33)+D11</f>
+        <f t="shared" si="3"/>
         <v>557</v>
       </c>
       <c r="E32" s="6">
-        <f>MIN(D32,E33)+E11</f>
+        <f t="shared" si="14"/>
         <v>620</v>
       </c>
       <c r="F32" s="6">
-        <f>MIN(E32,F33)+F11</f>
+        <f t="shared" si="15"/>
         <v>634</v>
       </c>
       <c r="G32" s="6">
-        <f>MIN(F32,G33)+G11</f>
+        <f t="shared" si="17"/>
         <v>659</v>
       </c>
       <c r="H32" s="6">
-        <f>MIN(G32,H33)+H11</f>
+        <f t="shared" si="18"/>
         <v>749</v>
       </c>
       <c r="I32" s="7">
-        <f>MIN(H32,I33)+I11</f>
+        <f t="shared" si="19"/>
         <v>709</v>
       </c>
       <c r="J32" s="6">
@@ -2591,43 +2597,43 @@
         <v>785</v>
       </c>
       <c r="K32" s="6">
-        <f>MIN(J32,K33)+K11</f>
+        <f t="shared" si="20"/>
         <v>829</v>
       </c>
       <c r="L32" s="6">
-        <f>MIN(K32,L33)+L11</f>
+        <f t="shared" si="20"/>
         <v>854</v>
       </c>
       <c r="M32" s="6">
-        <f>MIN(L32,M33)+M11</f>
+        <f t="shared" si="7"/>
         <v>848</v>
       </c>
       <c r="N32" s="6">
-        <f>MIN(M32,N33)+N11</f>
+        <f t="shared" si="8"/>
         <v>864</v>
       </c>
       <c r="O32" s="6">
-        <f>MIN(N32,O33)+O11</f>
+        <f t="shared" si="9"/>
         <v>912</v>
       </c>
       <c r="P32" s="6">
-        <f>MIN(O32,P33)+P11</f>
+        <f t="shared" si="10"/>
         <v>948</v>
       </c>
       <c r="Q32" s="6">
-        <f>MIN(P32,Q33)+Q11</f>
+        <f t="shared" si="16"/>
         <v>977</v>
       </c>
       <c r="R32" s="6">
-        <f>MIN(Q32,R33)+R11</f>
+        <f t="shared" si="11"/>
         <v>1012</v>
       </c>
       <c r="S32" s="6">
-        <f>MIN(R32,S33)+S11</f>
+        <f t="shared" si="12"/>
         <v>1066</v>
       </c>
       <c r="T32" s="7">
-        <f>MIN(S32,T33)+T11</f>
+        <f t="shared" si="13"/>
         <v>1115</v>
       </c>
     </row>
@@ -2637,35 +2643,35 @@
         <v>475</v>
       </c>
       <c r="B33" s="6">
-        <f>MIN(A33,B34)+B12</f>
+        <f t="shared" si="1"/>
         <v>499</v>
       </c>
       <c r="C33" s="6">
-        <f>MIN(B33,C34)+C12</f>
+        <f t="shared" si="2"/>
         <v>546</v>
       </c>
       <c r="D33" s="6">
-        <f>MIN(C33,D34)+D12</f>
+        <f t="shared" si="3"/>
         <v>535</v>
       </c>
       <c r="E33" s="6">
-        <f>MIN(D33,E34)+E12</f>
+        <f t="shared" si="14"/>
         <v>559</v>
       </c>
       <c r="F33" s="6">
-        <f>MIN(E33,F34)+F12</f>
+        <f t="shared" si="15"/>
         <v>590</v>
       </c>
       <c r="G33" s="6">
-        <f>MIN(F33,G34)+G12</f>
+        <f t="shared" si="17"/>
         <v>619</v>
       </c>
       <c r="H33" s="6">
-        <f>MIN(G33,H34)+H12</f>
+        <f t="shared" si="18"/>
         <v>650</v>
       </c>
       <c r="I33" s="6">
-        <f>MIN(H33,I34)+I12</f>
+        <f t="shared" si="19"/>
         <v>667</v>
       </c>
       <c r="J33" s="6">
@@ -2673,11 +2679,11 @@
         <v>748</v>
       </c>
       <c r="K33" s="6">
-        <f>MIN(J33,K34)+K12</f>
+        <f t="shared" si="20"/>
         <v>741</v>
       </c>
       <c r="L33" s="6">
-        <f>MIN(K33,L34)+L12</f>
+        <f t="shared" si="20"/>
         <v>782</v>
       </c>
       <c r="M33" s="8">
@@ -2697,19 +2703,19 @@
         <v>898</v>
       </c>
       <c r="Q33" s="6">
-        <f>MIN(P33,Q34)+Q12</f>
+        <f t="shared" si="16"/>
         <v>993</v>
       </c>
       <c r="R33" s="6">
-        <f>MIN(Q33,R34)+R12</f>
+        <f t="shared" si="11"/>
         <v>1046</v>
       </c>
       <c r="S33" s="6">
-        <f>MIN(R33,S34)+S12</f>
+        <f t="shared" si="12"/>
         <v>1121</v>
       </c>
       <c r="T33" s="7">
-        <f>MIN(S33,T34)+T12</f>
+        <f t="shared" si="13"/>
         <v>1161</v>
       </c>
     </row>
@@ -2719,35 +2725,35 @@
         <v>407</v>
       </c>
       <c r="B34" s="6">
-        <f>MIN(A34,B35)+B13</f>
+        <f t="shared" si="1"/>
         <v>431</v>
       </c>
       <c r="C34" s="6">
-        <f>MIN(B34,C35)+C13</f>
+        <f t="shared" si="2"/>
         <v>525</v>
       </c>
       <c r="D34" s="6">
-        <f>MIN(C34,D35)+D13</f>
+        <f t="shared" si="3"/>
         <v>511</v>
       </c>
       <c r="E34" s="6">
-        <f>MIN(D34,E35)+E13</f>
+        <f t="shared" si="14"/>
         <v>580</v>
       </c>
       <c r="F34" s="6">
-        <f>MIN(E34,F35)+F13</f>
+        <f t="shared" si="15"/>
         <v>521</v>
       </c>
       <c r="G34" s="6">
-        <f>MIN(F34,G35)+G13</f>
+        <f t="shared" si="17"/>
         <v>557</v>
       </c>
       <c r="H34" s="6">
-        <f>MIN(G34,H35)+H13</f>
+        <f t="shared" si="18"/>
         <v>628</v>
       </c>
       <c r="I34" s="6">
-        <f>MIN(H34,I35)+I13</f>
+        <f t="shared" si="19"/>
         <v>645</v>
       </c>
       <c r="J34" s="6">
@@ -2755,19 +2761,19 @@
         <v>654</v>
       </c>
       <c r="K34" s="6">
-        <f>MIN(J34,K35)+K13</f>
+        <f t="shared" si="20"/>
         <v>694</v>
       </c>
       <c r="L34" s="6">
-        <f>MIN(K34,L35)+L13</f>
+        <f t="shared" si="20"/>
         <v>748</v>
       </c>
       <c r="M34" s="6">
-        <f>MIN(L34,M35)+M13</f>
+        <f t="shared" ref="M34:N36" si="21">MIN(L34,M35)+M13</f>
         <v>783</v>
       </c>
       <c r="N34" s="12">
-        <f>MIN(M34,N35)+N13</f>
+        <f t="shared" si="21"/>
         <v>743</v>
       </c>
       <c r="O34" s="6">
@@ -2779,19 +2785,19 @@
         <v>882</v>
       </c>
       <c r="Q34" s="6">
-        <f>MIN(P34,Q35)+Q13</f>
+        <f t="shared" si="16"/>
         <v>900</v>
       </c>
       <c r="R34" s="6">
-        <f>MIN(Q34,R35)+R13</f>
+        <f t="shared" si="11"/>
         <v>987</v>
       </c>
       <c r="S34" s="6">
-        <f>MIN(R34,S35)+S13</f>
+        <f t="shared" si="12"/>
         <v>1054</v>
       </c>
       <c r="T34" s="7">
-        <f>MIN(S34,T35)+T13</f>
+        <f t="shared" si="13"/>
         <v>1073</v>
       </c>
     </row>
@@ -2801,35 +2807,35 @@
         <v>337</v>
       </c>
       <c r="B35" s="6">
-        <f>MIN(A35,B36)+B14</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="C35" s="6">
-        <f>MIN(B35,C36)+C14</f>
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
       <c r="D35" s="6">
-        <f>MIN(C35,D36)+D14</f>
+        <f t="shared" si="3"/>
         <v>482</v>
       </c>
       <c r="E35" s="6">
-        <f>MIN(D35,E36)+E14</f>
+        <f t="shared" si="14"/>
         <v>550</v>
       </c>
       <c r="F35" s="6">
-        <f>MIN(E35,F36)+F14</f>
+        <f t="shared" si="15"/>
         <v>485</v>
       </c>
       <c r="G35" s="6">
-        <f>MIN(F35,G36)+G14</f>
+        <f t="shared" si="17"/>
         <v>516</v>
       </c>
       <c r="H35" s="6">
-        <f>MIN(G35,H36)+H14</f>
+        <f t="shared" si="18"/>
         <v>545</v>
       </c>
       <c r="I35" s="6">
-        <f>MIN(H35,I36)+I14</f>
+        <f t="shared" si="19"/>
         <v>558</v>
       </c>
       <c r="J35" s="6">
@@ -2837,19 +2843,19 @@
         <v>612</v>
       </c>
       <c r="K35" s="6">
-        <f>MIN(J35,K36)+K14</f>
+        <f t="shared" si="20"/>
         <v>648</v>
       </c>
       <c r="L35" s="6">
-        <f>MIN(K35,L36)+L14</f>
+        <f t="shared" si="20"/>
         <v>702</v>
       </c>
       <c r="M35" s="6">
-        <f>MIN(L35,M36)+M14</f>
+        <f t="shared" si="21"/>
         <v>710</v>
       </c>
       <c r="N35" s="7">
-        <f>MIN(M35,N36)+N14</f>
+        <f t="shared" si="21"/>
         <v>705</v>
       </c>
       <c r="O35" s="6">
@@ -2861,19 +2867,19 @@
         <v>804</v>
       </c>
       <c r="Q35" s="6">
-        <f>MIN(P35,Q36)+Q14</f>
+        <f t="shared" si="16"/>
         <v>819</v>
       </c>
       <c r="R35" s="6">
-        <f>MIN(Q35,R36)+R14</f>
+        <f t="shared" si="11"/>
         <v>888</v>
       </c>
       <c r="S35" s="6">
-        <f>MIN(R35,S36)+S14</f>
+        <f t="shared" si="12"/>
         <v>959</v>
       </c>
       <c r="T35" s="7">
-        <f>MIN(S35,T36)+T14</f>
+        <f t="shared" si="13"/>
         <v>994</v>
       </c>
     </row>
@@ -2883,35 +2889,35 @@
         <v>308</v>
       </c>
       <c r="B36" s="6">
-        <f>MIN(A36,B37)+B15</f>
+        <f t="shared" si="1"/>
         <v>394</v>
       </c>
       <c r="C36" s="6">
-        <f>MIN(B36,C37)+C15</f>
+        <f t="shared" si="2"/>
         <v>406</v>
       </c>
       <c r="D36" s="6">
-        <f>MIN(C36,D37)+D15</f>
+        <f t="shared" si="3"/>
         <v>488</v>
       </c>
       <c r="E36" s="6">
-        <f>MIN(D36,E37)+E15</f>
+        <f t="shared" si="14"/>
         <v>463</v>
       </c>
       <c r="F36" s="6">
-        <f>MIN(E36,F37)+F15</f>
+        <f t="shared" si="15"/>
         <v>434</v>
       </c>
       <c r="G36" s="6">
-        <f>MIN(F36,G37)+G15</f>
+        <f t="shared" si="17"/>
         <v>480</v>
       </c>
       <c r="H36" s="6">
-        <f>MIN(G36,H37)+H15</f>
+        <f t="shared" si="18"/>
         <v>499</v>
       </c>
       <c r="I36" s="6">
-        <f>MIN(H36,I37)+I15</f>
+        <f t="shared" si="19"/>
         <v>526</v>
       </c>
       <c r="J36" s="6">
@@ -2919,19 +2925,19 @@
         <v>569</v>
       </c>
       <c r="K36" s="6">
-        <f>MIN(J36,K37)+K15</f>
+        <f t="shared" si="20"/>
         <v>632</v>
       </c>
       <c r="L36" s="6">
-        <f>MIN(K36,L37)+L15</f>
+        <f t="shared" si="20"/>
         <v>675</v>
       </c>
       <c r="M36" s="6">
-        <f>MIN(L36,M37)+M15</f>
+        <f t="shared" si="21"/>
         <v>657</v>
       </c>
       <c r="N36" s="6">
-        <f>MIN(M36,N37)+N15</f>
+        <f t="shared" si="21"/>
         <v>686</v>
       </c>
       <c r="O36" s="6">
@@ -2943,19 +2949,19 @@
         <v>767</v>
       </c>
       <c r="Q36" s="6">
-        <f>MIN(P36,Q37)+Q15</f>
+        <f t="shared" si="16"/>
         <v>813</v>
       </c>
       <c r="R36" s="6">
-        <f>MIN(Q36,R37)+R15</f>
+        <f t="shared" si="11"/>
         <v>829</v>
       </c>
       <c r="S36" s="6">
-        <f>MIN(R36,S37)+S15</f>
+        <f t="shared" si="12"/>
         <v>891</v>
       </c>
       <c r="T36" s="7">
-        <f>MIN(S36,T37)+T15</f>
+        <f t="shared" si="13"/>
         <v>989</v>
       </c>
       <c r="X36" s="13">
@@ -2968,79 +2974,79 @@
         <v>288</v>
       </c>
       <c r="B37" s="6">
-        <f>MIN(A37,B38)+B16</f>
+        <f t="shared" si="1"/>
         <v>332</v>
       </c>
       <c r="C37" s="6">
-        <f>MIN(B37,C38)+C16</f>
+        <f t="shared" si="2"/>
         <v>342</v>
       </c>
       <c r="D37" s="6">
-        <f>MIN(C37,D38)+D16</f>
+        <f t="shared" si="3"/>
         <v>391</v>
       </c>
       <c r="E37" s="6">
-        <f>MIN(D37,E38)+E16</f>
+        <f t="shared" si="14"/>
         <v>392</v>
       </c>
       <c r="F37" s="6">
-        <f>MIN(E37,F38)+F16</f>
+        <f t="shared" si="15"/>
         <v>414</v>
       </c>
       <c r="G37" s="6">
-        <f>MIN(F37,G38)+G16</f>
+        <f t="shared" si="17"/>
         <v>460</v>
       </c>
       <c r="H37" s="6">
-        <f>MIN(G37,H38)+H16</f>
+        <f t="shared" si="18"/>
         <v>459</v>
       </c>
       <c r="I37" s="6">
-        <f>MIN(H37,I38)+I16</f>
+        <f t="shared" si="19"/>
         <v>522</v>
       </c>
       <c r="J37" s="6">
-        <f>MIN(I37)+J16</f>
+        <f t="shared" ref="J37:T37" si="22">MIN(I37)+J16</f>
         <v>532</v>
       </c>
       <c r="K37" s="6">
-        <f>MIN(J37)+K16</f>
+        <f t="shared" si="22"/>
         <v>549</v>
       </c>
       <c r="L37" s="6">
-        <f>MIN(K37)+L16</f>
+        <f t="shared" si="22"/>
         <v>613</v>
       </c>
       <c r="M37" s="6">
-        <f>MIN(L37)+M16</f>
+        <f t="shared" si="22"/>
         <v>644</v>
       </c>
       <c r="N37" s="6">
-        <f>MIN(M37)+N16</f>
+        <f t="shared" si="22"/>
         <v>675</v>
       </c>
       <c r="O37" s="6">
-        <f>MIN(N37)+O16</f>
+        <f t="shared" si="22"/>
         <v>757</v>
       </c>
       <c r="P37" s="6">
-        <f>MIN(O37)+P16</f>
+        <f t="shared" si="22"/>
         <v>831</v>
       </c>
       <c r="Q37" s="6">
-        <f>MIN(P37)+Q16</f>
+        <f t="shared" si="22"/>
         <v>894</v>
       </c>
       <c r="R37" s="6">
-        <f>MIN(Q37)+R16</f>
+        <f t="shared" si="22"/>
         <v>958</v>
       </c>
       <c r="S37" s="6">
-        <f>MIN(R37)+S16</f>
+        <f t="shared" si="22"/>
         <v>1004</v>
       </c>
       <c r="T37" s="7">
-        <f>MIN(S37)+T16</f>
+        <f t="shared" si="22"/>
         <v>1030</v>
       </c>
       <c r="X37" s="13">
@@ -3053,35 +3059,35 @@
         <v>224</v>
       </c>
       <c r="B38" s="6">
-        <f>MIN(A38,B39)+B17</f>
+        <f t="shared" si="1"/>
         <v>234</v>
       </c>
       <c r="C38" s="6">
-        <f>MIN(B38,C39)+C17</f>
+        <f t="shared" si="2"/>
         <v>304</v>
       </c>
       <c r="D38" s="6">
-        <f>MIN(C38,D39)+D17</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="E38" s="6">
-        <f>MIN(D38,E39)+E17</f>
+        <f t="shared" si="14"/>
         <v>367</v>
       </c>
       <c r="F38" s="6">
-        <f>MIN(E38,F39)+F17</f>
+        <f t="shared" si="15"/>
         <v>378</v>
       </c>
       <c r="G38" s="6">
-        <f>MIN(F38,G39)+G17</f>
+        <f t="shared" si="17"/>
         <v>454</v>
       </c>
       <c r="H38" s="6">
-        <f>MIN(G38,H39)+H17</f>
+        <f t="shared" si="18"/>
         <v>427</v>
       </c>
       <c r="I38" s="7">
-        <f>MIN(H38,I39)+I17</f>
+        <f t="shared" si="19"/>
         <v>457</v>
       </c>
       <c r="J38" s="6"/>
@@ -3102,35 +3108,35 @@
         <v>165</v>
       </c>
       <c r="B39" s="6">
-        <f>MIN(A39,B40)+B18</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="C39" s="6">
-        <f>MIN(B39,C40)+C18</f>
+        <f t="shared" si="2"/>
         <v>229</v>
       </c>
       <c r="D39" s="6">
-        <f>MIN(C39,D40)+D18</f>
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
       <c r="E39" s="6">
-        <f>MIN(D39,E40)+E18</f>
+        <f t="shared" si="14"/>
         <v>278</v>
       </c>
       <c r="F39" s="6">
-        <f>MIN(E39,F40)+F18</f>
+        <f t="shared" si="15"/>
         <v>323</v>
       </c>
       <c r="G39" s="6">
-        <f>MIN(F39,G40)+G18</f>
+        <f t="shared" si="17"/>
         <v>415</v>
       </c>
       <c r="H39" s="6">
-        <f>MIN(G39,H40)+H18</f>
+        <f t="shared" si="18"/>
         <v>382</v>
       </c>
       <c r="I39" s="7">
-        <f>MIN(H39,I40)+I18</f>
+        <f t="shared" si="19"/>
         <v>451</v>
       </c>
       <c r="J39" s="6"/>
@@ -3151,35 +3157,35 @@
         <v>73</v>
       </c>
       <c r="B40" s="6">
-        <f>MIN(A40,B41)+B19</f>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="C40" s="6">
-        <f>MIN(B40,C41)+C19</f>
+        <f t="shared" si="2"/>
         <v>151</v>
       </c>
       <c r="D40" s="6">
-        <f>MIN(C40,D41)+D19</f>
+        <f t="shared" si="3"/>
         <v>216</v>
       </c>
       <c r="E40" s="6">
-        <f>MIN(D40,E41)+E19</f>
+        <f t="shared" si="14"/>
         <v>238</v>
       </c>
       <c r="F40" s="6">
-        <f>MIN(E40,F41)+F19</f>
+        <f t="shared" si="15"/>
         <v>255</v>
       </c>
       <c r="G40" s="6">
-        <f>MIN(F40,G41)+G19</f>
+        <f t="shared" si="17"/>
         <v>320</v>
       </c>
       <c r="H40" s="6">
-        <f>MIN(G40,H41)+H19</f>
+        <f t="shared" si="18"/>
         <v>360</v>
       </c>
       <c r="I40" s="7">
-        <f>MIN(H40,I41)+I19</f>
+        <f t="shared" si="19"/>
         <v>370</v>
       </c>
       <c r="J40" s="6"/>
@@ -3203,27 +3209,27 @@
         <v>125</v>
       </c>
       <c r="C41" s="8">
-        <f t="shared" ref="C41:T41" si="1">B41+C20</f>
+        <f t="shared" ref="C41:H41" si="23">B41+C20</f>
         <v>142</v>
       </c>
       <c r="D41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="23"/>
         <v>234</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="23"/>
         <v>325</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="23"/>
         <v>351</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="23"/>
         <v>420</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="23"/>
         <v>488</v>
       </c>
       <c r="I41" s="9">

</xml_diff>